<commit_message>
Add other Province, Wuhan more precise
</commit_message>
<xml_diff>
--- a/Wuhan_Data.xlsx
+++ b/Wuhan_Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86150\.spyder-py3\projects\MCM-ICM2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED7502A-F9A4-4456-BC78-10CDBD338D2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5155CED1-192E-41A6-AD90-16358016B5E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0428A156-C80A-40D8-92F7-D7D05A657BE1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{0428A156-C80A-40D8-92F7-D7D05A657BE1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Wuhan" sheetId="1" r:id="rId1"/>
+    <sheet name="Hubei" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Death</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,6 +43,10 @@
   </si>
   <si>
     <t>Recover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cofirmed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -408,6 +413,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBCC87C-0F16-440C-B066-8A605449AE9F}">
   <dimension ref="A1:C22"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>198</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>258</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>363</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>425</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>495</v>
+      </c>
+      <c r="B10">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>572</v>
+      </c>
+      <c r="B11">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>618</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>698</v>
+      </c>
+      <c r="B13">
+        <v>63</v>
+      </c>
+      <c r="C13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1590</v>
+      </c>
+      <c r="B14">
+        <v>85</v>
+      </c>
+      <c r="C14">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1905</v>
+      </c>
+      <c r="B15">
+        <v>104</v>
+      </c>
+      <c r="C15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2261</v>
+      </c>
+      <c r="B16">
+        <v>129</v>
+      </c>
+      <c r="C16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2639</v>
+      </c>
+      <c r="B17">
+        <v>159</v>
+      </c>
+      <c r="C17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3215</v>
+      </c>
+      <c r="B18">
+        <v>192</v>
+      </c>
+      <c r="C18">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>4109</v>
+      </c>
+      <c r="B19">
+        <v>224</v>
+      </c>
+      <c r="C19">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5142</v>
+      </c>
+      <c r="B20">
+        <v>265</v>
+      </c>
+      <c r="C20">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>6384</v>
+      </c>
+      <c r="B21">
+        <v>313</v>
+      </c>
+      <c r="C21">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>8351</v>
+      </c>
+      <c r="B22">
+        <v>362</v>
+      </c>
+      <c r="C22">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8648DC6-444E-4BAC-8A83-515610F449DC}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
@@ -416,7 +680,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -427,233 +691,178 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>41</v>
+        <v>270</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>45</v>
+        <v>375</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>62</v>
+        <v>444</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>121</v>
+        <v>549</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>198</v>
+        <v>729</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>258</v>
+        <v>1052</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>363</v>
+        <v>1423</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="C8">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>425</v>
+        <v>2714</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="C9">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>495</v>
+        <v>3554</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="C10">
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>572</v>
+        <v>4586</v>
       </c>
       <c r="B11">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="C11">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>618</v>
+        <v>5806</v>
       </c>
       <c r="B12">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C12">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>698</v>
+        <v>7153</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>249</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1590</v>
+        <v>9074</v>
       </c>
       <c r="B14">
-        <v>85</v>
+        <v>294</v>
       </c>
       <c r="C14">
-        <v>42</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1905</v>
+        <v>11177</v>
       </c>
       <c r="B15">
-        <v>104</v>
+        <v>350</v>
       </c>
       <c r="C15">
-        <v>42</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2261</v>
+        <v>13522</v>
       </c>
       <c r="B16">
-        <v>129</v>
+        <v>414</v>
       </c>
       <c r="C16">
-        <v>49</v>
+        <v>396</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>2639</v>
+        <v>16678</v>
       </c>
       <c r="B17">
-        <v>159</v>
+        <v>479</v>
       </c>
       <c r="C17">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>3215</v>
-      </c>
-      <c r="B18">
-        <v>192</v>
-      </c>
-      <c r="C18">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>4109</v>
-      </c>
-      <c r="B19">
-        <v>224</v>
-      </c>
-      <c r="C19">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>5142</v>
-      </c>
-      <c r="B20">
-        <v>265</v>
-      </c>
-      <c r="C20">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>6384</v>
-      </c>
-      <c r="B21">
-        <v>313</v>
-      </c>
-      <c r="C21">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>8351</v>
-      </c>
-      <c r="B22">
-        <v>362</v>
-      </c>
-      <c r="C22">
-        <v>335</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>